<commit_message>
Several percentages fixed for new tables. not done yet.
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table3.xlsx
+++ b/data/maingraphs-code-size-table3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
@@ -506,8 +506,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="329">
+  <cellStyleXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -852,7 +854,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="329">
+  <cellStyles count="331">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1017,6 +1019,7 @@
     <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1181,6 +1184,7 @@
     <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1512,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3803,7 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="N94" sqref="A84:N94"/>
     </sheetView>
   </sheetViews>
@@ -8388,7 +8392,7 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <f>B26-B$25</f>
+        <f t="shared" ref="B37:B45" si="4">B26-B$25</f>
         <v>6863</v>
       </c>
       <c r="G37">
@@ -8401,11 +8405,11 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <f>B27-B$25</f>
+        <f t="shared" si="4"/>
         <v>7139</v>
       </c>
       <c r="C38">
-        <f>B38-B$37</f>
+        <f t="shared" ref="C38:C45" si="5">B38-B$37</f>
         <v>276</v>
       </c>
       <c r="D38">
@@ -8430,23 +8434,23 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <f>B28-B$25</f>
+        <f t="shared" si="4"/>
         <v>7961</v>
       </c>
       <c r="C39">
-        <f>B39-B$37</f>
+        <f t="shared" si="5"/>
         <v>1098</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:D45" si="4">B39-B38</f>
+        <f t="shared" ref="D39:D45" si="6">B39-B38</f>
         <v>822</v>
       </c>
       <c r="E39" s="6">
-        <f t="shared" ref="E39:E45" si="5">P16</f>
+        <f t="shared" ref="E39:E45" si="7">P16</f>
         <v>-0.27840895795886378</v>
       </c>
       <c r="F39" s="7">
-        <f t="shared" ref="F39:F45" si="6">-C39/E39/1000</f>
+        <f t="shared" ref="F39:F45" si="8">-C39/E39/1000</f>
         <v>3.9438386180168621</v>
       </c>
       <c r="G39" s="5">
@@ -8459,23 +8463,23 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <f>B29-B$25</f>
+        <f t="shared" si="4"/>
         <v>9229</v>
       </c>
       <c r="C40">
-        <f>B40-B$37</f>
+        <f t="shared" si="5"/>
         <v>2366</v>
       </c>
       <c r="D40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1268</v>
       </c>
       <c r="E40" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.33096607956972018</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.1487688498953457</v>
       </c>
       <c r="G40" s="5">
@@ -8488,23 +8492,23 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <f>B30-B$25</f>
+        <f t="shared" si="4"/>
         <v>12511</v>
       </c>
       <c r="C41">
-        <f>B41-B$37</f>
+        <f t="shared" si="5"/>
         <v>5648</v>
       </c>
       <c r="D41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3282</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.33393537565693232</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>16.913452157888354</v>
       </c>
       <c r="G41" s="5">
@@ -8517,23 +8521,23 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <f>B31-B$25</f>
+        <f t="shared" si="4"/>
         <v>12955</v>
       </c>
       <c r="C42">
-        <f>B42-B$37</f>
+        <f t="shared" si="5"/>
         <v>6092</v>
       </c>
       <c r="D42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>444</v>
       </c>
       <c r="E42" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.34318379027484597</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17.751421170332939</v>
       </c>
       <c r="G42" s="5">
@@ -8546,23 +8550,23 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <f>B32-B$25</f>
+        <f t="shared" si="4"/>
         <v>12935</v>
       </c>
       <c r="C43">
-        <f>B43-B$37</f>
+        <f t="shared" si="5"/>
         <v>6072</v>
       </c>
       <c r="D43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-20</v>
       </c>
       <c r="E43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.38698535812947649</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>15.690516120169196</v>
       </c>
       <c r="G43" s="5">
@@ -8575,23 +8579,23 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <f>B33-B$25</f>
+        <f t="shared" si="4"/>
         <v>13001</v>
       </c>
       <c r="C44">
-        <f>B44-B$37</f>
+        <f t="shared" si="5"/>
         <v>6138</v>
       </c>
       <c r="D44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="E44" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.39196295440146989</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>15.659643165443448</v>
       </c>
       <c r="G44" s="5">
@@ -8604,23 +8608,23 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <f>B34-B$25</f>
+        <f t="shared" si="4"/>
         <v>13549</v>
       </c>
       <c r="C45">
-        <f>B45-B$37</f>
+        <f t="shared" si="5"/>
         <v>6686</v>
       </c>
       <c r="D45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>548</v>
       </c>
       <c r="E45" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.39741178598256155</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>16.823859371632683</v>
       </c>
       <c r="G45" s="5">

</xml_diff>